<commit_message>
SSIM Docs and Data Types wip
</commit_message>
<xml_diff>
--- a/Docs/SpreadSheets/SSIM Data Types.xlsx
+++ b/Docs/SpreadSheets/SSIM Data Types.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Pacio\Development\SSIM Proto\Docs\SpreadSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BC9FFB-9AB9-4500-939C-74CE561667A1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D9A329-2CCF-47FA-9105-90F25DC0DF85}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12075" tabRatio="688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Intrinsic" sheetId="29" r:id="rId1"/>
-    <sheet name="Money" sheetId="30" r:id="rId2"/>
+    <sheet name="Base" sheetId="32" r:id="rId1"/>
+    <sheet name="Intrinsic" sheetId="29" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="31" r:id="rId3"/>
+    <sheet name="Money" sheetId="30" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
-  <si>
-    <t>Id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="128">
   <si>
     <t>Name</t>
   </si>
@@ -338,6 +337,147 @@
   </si>
   <si>
     <t>Consider XML buiult in data types</t>
+  </si>
+  <si>
+    <t>Base Data Types</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>Bits</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Blob</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>SSIM_DTB_Base | SSIM_DTB_DateTime</t>
+  </si>
+  <si>
+    <t>SSIM_DTB_Base | SSIM_DTB_Numeric</t>
+  </si>
+  <si>
+    <t>A string of UTF-8 encoded charcaters</t>
+  </si>
+  <si>
+    <t>SSIM_DTB_Base | SSIM_DTB_String</t>
+  </si>
+  <si>
+    <t>SSIM_DTB_Base | SSIM_DTB_Blob</t>
+  </si>
+  <si>
+    <t>SSIM_DTB_Base | SSIM_DTB_File</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>A sequence of binary bytes - a 'blob' of data</t>
+  </si>
+  <si>
+    <t>A file in binary form</t>
+  </si>
+  <si>
+    <t>The "." and ':' separators can be any non digit characters</t>
+  </si>
+  <si>
+    <t>A number as commonly understood</t>
+  </si>
+  <si>
+    <t>A date and optionally time in string numeric form year first {CC}YY.MM.DD{ HH:MM{:SS}}</t>
+  </si>
+  <si>
+    <t>Base 10 number, as per a Json Number</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Used when the SID description from the Facts Directories completely defines the data and there is no need to store anything apart from the SID e.g. a country shown externally as the country name in the human language of choice, or a 3 letter country code, or a 2 letters cod according to formatting options</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Base data types apply to one item of data. They intuitive and suitable for many simple cases e.g. most facts in the SSIM Facts Directories</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A SID is an SSIM Id used to provide standardised semantic description of an item of data</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The Bits column is only relevant to a programmer. The Constants quoted are defined in ConstantsSSIM.inc</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -346,9 +486,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,6 +497,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -385,13 +533,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -673,44 +831,187 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988DF991-EDC9-4A2B-9317-26F5CEC72EF1}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="8.73046875" customWidth="1"/>
+    <col min="2" max="2" width="88.33203125" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02E59163-2B59-4D34-9718-A749A296049A}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:J89"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.9296875" customWidth="1"/>
-    <col min="2" max="2" width="12.86328125" customWidth="1"/>
-    <col min="5" max="6" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="78.06640625" customWidth="1"/>
-    <col min="8" max="8" width="19.3984375" customWidth="1"/>
-    <col min="9" max="9" width="19.9296875" customWidth="1"/>
-    <col min="10" max="10" width="11.265625" customWidth="1"/>
+    <col min="1" max="1" width="12.86328125" customWidth="1"/>
+    <col min="4" max="5" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="78.06640625" customWidth="1"/>
+    <col min="7" max="7" width="19.3984375" customWidth="1"/>
+    <col min="8" max="8" width="19.9296875" customWidth="1"/>
+    <col min="9" max="9" width="11.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="E2" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
         <v>78</v>
@@ -722,490 +1023,490 @@
         <v>80</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="H3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" s="3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="3">
         <f xml:space="preserve"> -2147483648</f>
         <v>-2147483648</v>
       </c>
-      <c r="F4" s="2">
+      <c r="E4" s="2">
         <f>2147483647</f>
         <v>2147483647</v>
       </c>
+      <c r="F4" t="s">
+        <v>81</v>
+      </c>
       <c r="G4" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="H4" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="I4" t="s">
-        <v>86</v>
-      </c>
-      <c r="J4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" s="3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="3">
         <v>0</v>
       </c>
-      <c r="F5" s="2">
+      <c r="E5" s="2">
         <f>2^32-1</f>
         <v>4294967295</v>
       </c>
+      <c r="F5" t="s">
+        <v>89</v>
+      </c>
       <c r="G5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H5" t="s">
-        <v>84</v>
-      </c>
-      <c r="I5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" t="s">
         <v>92</v>
       </c>
-      <c r="J5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>97</v>
-      </c>
-      <c r="I6" t="s">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="D7" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B10" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{985696F7-DD0B-4931-AD34-ADB48DA2CB86}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2865CB-771F-4501-9A62-2008850DDC05}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
SSIM Docs and Data Types Wip 2
</commit_message>
<xml_diff>
--- a/Docs/SpreadSheets/SSIM Data Types.xlsx
+++ b/Docs/SpreadSheets/SSIM Data Types.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Pacio\Development\SSIM Proto\Docs\SpreadSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D9A329-2CCF-47FA-9105-90F25DC0DF85}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B64B40-03B2-4F78-8EE1-796337E3030C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12075" tabRatio="688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12075" tabRatio="688" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="32" r:id="rId1"/>
-    <sheet name="Intrinsic" sheetId="29" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="31" r:id="rId3"/>
-    <sheet name="Money" sheetId="30" r:id="rId4"/>
+    <sheet name="Json" sheetId="33" r:id="rId2"/>
+    <sheet name="Std" sheetId="29" r:id="rId3"/>
+    <sheet name="XML" sheetId="31" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="145">
   <si>
     <t>Name</t>
   </si>
@@ -315,9 +315,6 @@
     <t>INT unsigned</t>
   </si>
   <si>
-    <t>Simple Numeric Data Types - One Item</t>
-  </si>
-  <si>
     <t>* const TETN_Integer       =  1; # xbrli:integerItemType               9</t>
   </si>
   <si>
@@ -342,36 +339,12 @@
     <t>Base Data Types</t>
   </si>
   <si>
-    <t>Null</t>
-  </si>
-  <si>
     <t>Bits</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>DateTime</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>Blob</t>
-  </si>
-  <si>
-    <t>File</t>
-  </si>
-  <si>
-    <t>SSIM_DTB_Base | SSIM_DTB_DateTime</t>
-  </si>
-  <si>
-    <t>SSIM_DTB_Base | SSIM_DTB_Numeric</t>
-  </si>
-  <si>
     <t>A string of UTF-8 encoded charcaters</t>
   </si>
   <si>
@@ -384,31 +357,232 @@
     <t>SSIM_DTB_Base | SSIM_DTB_File</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>A sequence of binary bytes - a 'blob' of data</t>
   </si>
   <si>
     <t>A file in binary form</t>
   </si>
   <si>
-    <t>The "." and ':' separators can be any non digit characters</t>
-  </si>
-  <si>
-    <t>A number as commonly understood</t>
-  </si>
-  <si>
-    <t>A date and optionally time in string numeric form year first {CC}YY.MM.DD{ HH:MM{:SS}}</t>
-  </si>
-  <si>
-    <t>Base 10 number, as per a Json Number</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
     <t>Used when the SID description from the Facts Directories completely defines the data and there is no need to store anything apart from the SID e.g. a country shown externally as the country name in the human language of choice, or a 3 letter country code, or a 2 letters cod according to formatting options</t>
+  </si>
+  <si>
+    <t>Json Data Types</t>
+  </si>
+  <si>
+    <t>https://www.json.org/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">An </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>object</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is an unordered set of name/value pairs. An object begins with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7.5"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(left brace)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and ends with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7.5"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(right brace)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Each name is followed by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7.5"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(colon)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and the name/value pairs are separated by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7.5"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(comma)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is a sequence of zero or more Unicode characters, wrapped in double quotes, using backslash escapes. A character is represented as a single character string. A string is very much like a C or Java string.</t>
+    </r>
+  </si>
+  <si>
+    <t>XML Data Types</t>
+  </si>
+  <si>
+    <t>Base data types apply to one item of data. They are intuitive and suitable for many simple cases e.g. most facts in the SSIM Facts Directories</t>
   </si>
   <si>
     <r>
@@ -420,7 +594,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>a.</t>
+      <t>b.</t>
     </r>
     <r>
       <rPr>
@@ -430,7 +604,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Base data types apply to one item of data. They intuitive and suitable for many simple cases e.g. most facts in the SSIM Facts Directories</t>
+      <t xml:space="preserve"> The Bits column is only relevant to a programmer. The Constants quoted are defined in ConstantsSSIM.inc</t>
     </r>
   </si>
   <si>
@@ -443,7 +617,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>b.</t>
+      <t>a.</t>
     </r>
     <r>
       <rPr>
@@ -455,6 +629,48 @@
       </rPr>
       <t xml:space="preserve"> A SID is an SSIM Id used to provide standardised semantic description of an item of data</t>
     </r>
+  </si>
+  <si>
+    <t>The Json data trypes are defined at</t>
+  </si>
+  <si>
+    <t>Standard (Std) Data Types</t>
+  </si>
+  <si>
+    <t>The Standard Data Types are more precise or efficient than the Base or Json ones, more IT or DB oriented, suitable for use with apps developed by programmers.</t>
+  </si>
+  <si>
+    <t>Base.Null</t>
+  </si>
+  <si>
+    <t>Base.Number</t>
+  </si>
+  <si>
+    <t>Base.DateTime</t>
+  </si>
+  <si>
+    <t>Base.String</t>
+  </si>
+  <si>
+    <t>Base.Blob</t>
+  </si>
+  <si>
+    <t>Base.File</t>
+  </si>
+  <si>
+    <t>Json.Number</t>
+  </si>
+  <si>
+    <t>Json.String</t>
+  </si>
+  <si>
+    <t>Json.Object</t>
+  </si>
+  <si>
+    <t>Json.Array</t>
+  </si>
+  <si>
+    <t>An array is an ordered collection of values. An array begins with [ (left bracket) and ends with ] (right bracket). Values are separated by , (comma).</t>
   </si>
   <si>
     <r>
@@ -466,6 +682,61 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A value can be a string in double quotes, or a number, or "true" or "false" or "null", or an object or an array. These structures can be nested.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> For more re digits, hex digits, and ws (white space) see https://www.json.org/</t>
+    </r>
+  </si>
+  <si>
+    <t>SSIM_DTB_Base | SSIM_DTB_DateTime | SSIM_DTB_TextData</t>
+  </si>
+  <si>
+    <t>A base 10 number as commonly understood in text form, like a Json Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CC = 2 digit Century, YY  = 2 digit Year, MM = 2 digit Month 01 to 12, DD = 2 digit Day of the month 01 to 31, HH = Hour of the day 00 to 23, MM = Minute of the hour 00 to 59, SS = Second of the minute 00 to 59</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>c.</t>
     </r>
     <r>
@@ -476,8 +747,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> The Bits column is only relevant to a programmer. The Constants quoted are defined in ConstantsSSIM.inc</t>
-    </r>
+      <t xml:space="preserve"> For a DateTime the "." and ':' separators can be any non digit characters, sections enclosed within {}s are optional, and</t>
+    </r>
+  </si>
+  <si>
+    <t>A UTC/GMT date and optionally time in text numeric form year first CCYY.MM.DD{ HH:MM{:SS}}</t>
+  </si>
+  <si>
+    <t>SSIM_DTB_Json | SSIM_DTB_String | SSIM_DTB_TextData</t>
+  </si>
+  <si>
+    <t>SSIM_DTB_Json | SSIM_DTB_Object | SSIM_DTB_TextData</t>
+  </si>
+  <si>
+    <t>SSIM_DTB_Json | SSIM_DTB_Array | SSIM_DTB_TextData</t>
+  </si>
+  <si>
+    <t>SSIM_DTB_Json | SSIM_DTB_Number | SSIM_DTB_TextData</t>
+  </si>
+  <si>
+    <t>SSIM_DTB_Base | SSIM_DTB_Number | SSIM_DTB_TextData</t>
   </si>
 </sst>
 </file>
@@ -488,7 +777,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,6 +800,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -529,18 +846,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -551,9 +866,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -567,6 +897,255 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>10</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>10</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3417580</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1520200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13" descr="https://www.json.org/number.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52F975F1-63FE-41B8-93EB-DC815BAE24EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="871548" y="904885"/>
+          <a:ext cx="3417570" cy="1520190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>14298</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>238130</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3431868</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2598425</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14" descr="https://www.json.org/string.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B3A19C5-11A7-40B0-94F1-010795BD6A88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="885836" y="2809880"/>
+          <a:ext cx="3417570" cy="2360295"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28585</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>195276</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3446155</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>841071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15" descr="https://www.json.org/object.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA69D67C-0194-41E9-8D8F-711E7FED393D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="900123" y="5238764"/>
+          <a:ext cx="3417570" cy="645795"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19060</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>204787</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3436630</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>850582</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16" descr="https://www.json.org/array.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C9B94C1-7A4A-4440-9375-0838900A13CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="890598" y="6176962"/>
+          <a:ext cx="3417570" cy="645795"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -835,138 +1414,137 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.73046875" customWidth="1"/>
-    <col min="2" max="2" width="88.33203125" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.265625" customWidth="1"/>
+    <col min="1" max="1" width="12.59765625" customWidth="1"/>
+    <col min="2" max="2" width="50.46484375" customWidth="1"/>
+    <col min="3" max="3" width="88.33203125" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="42.75" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" t="s">
         <v>103</v>
       </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" t="s">
         <v>105</v>
       </c>
-      <c r="B5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="C10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" t="s">
         <v>106</v>
       </c>
-      <c r="B6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="C11" t="s">
         <v>108</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
         <v>117</v>
       </c>
-      <c r="D8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" t="s">
-        <v>118</v>
-      </c>
-      <c r="D9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1" t="s">
+        <v>137</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -975,17 +1553,133 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA7A8A1-3F59-4D4D-B5F1-02A309C4C2EA}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="12.19921875" customWidth="1"/>
+    <col min="2" max="2" width="48.59765625" customWidth="1"/>
+    <col min="3" max="3" width="82.53125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="13"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="131.25" customHeight="1">
+      <c r="A6" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="210" customHeight="1">
+      <c r="A7" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="73.150000000000006" customHeight="1">
+      <c r="A8" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="72.75" customHeight="1">
+      <c r="A9" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="12"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="10"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="10"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{5E666966-2E29-4258-B58A-E2635D5C61CE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02E59163-2B59-4D34-9718-A749A296049A}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:I89"/>
+  <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="12.86328125" customWidth="1"/>
     <col min="4" max="5" width="15.86328125" bestFit="1" customWidth="1"/>
@@ -995,525 +1689,530 @@
     <col min="9" max="9" width="11.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D2" s="4" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="9"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="9"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="D5" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B6" t="s">
         <v>77</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C6" t="s">
         <v>78</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D6" t="s">
         <v>79</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E6" t="s">
         <v>80</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F6" t="s">
         <v>76</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G6" t="s">
         <v>82</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H6" t="s">
         <v>84</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D7" s="3">
         <f xml:space="preserve"> -2147483648</f>
         <v>-2147483648</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E7" s="2">
         <f>2147483647</f>
         <v>2147483647</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F7" t="s">
         <v>81</v>
       </c>
-      <c r="G4" t="s">
-        <v>97</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="G7" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" t="s">
         <v>85</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D8" s="3">
         <v>0</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E8" s="2">
         <f>2^32-1</f>
         <v>4294967295</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F8" t="s">
         <v>89</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G8" t="s">
         <v>83</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>96</v>
-      </c>
-      <c r="H6" t="s">
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="C7" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A78" t="s">
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A82" t="s">
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A83" t="s">
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A85" t="s">
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A86" t="s">
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A87" t="s">
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A88" t="s">
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A89" t="s">
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{985696F7-DD0B-4931-AD34-ADB48DA2CB86}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2865CB-771F-4501-9A62-2008850DDC05}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>